<commit_message>
:hammer: Data con MuteFire
</commit_message>
<xml_diff>
--- a/Diarizacion.xlsx
+++ b/Diarizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C578B5-5953-4ED3-8080-ABF0D09525F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8758650F-D899-4B69-B8AF-D54FA87B674C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12345" activeTab="1" xr2:uid="{0224F83C-D3BE-49E4-82C2-87DC9D19A8C8}"/>
   </bookViews>
@@ -37,23 +37,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="72">
   <si>
     <t>177 MB</t>
   </si>
   <si>
-    <t>455 MB</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>861 MB</t>
   </si>
   <si>
-    <t>17 min</t>
-  </si>
-  <si>
     <t>CPU</t>
   </si>
   <si>
@@ -145,6 +136,123 @@
   </si>
   <si>
     <t>FRECUENCIA DE MUESTREO</t>
+  </si>
+  <si>
+    <t>OBSERVACIONES</t>
+  </si>
+  <si>
+    <t>Minuto 7 se pierde el speaker</t>
+  </si>
+  <si>
+    <t>244.83 segundos</t>
+  </si>
+  <si>
+    <t>237.55 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 235.85 segundos</t>
+  </si>
+  <si>
+    <t>236.70 segundos</t>
+  </si>
+  <si>
+    <t>238.03 segundos</t>
+  </si>
+  <si>
+    <t>234.26 segundos</t>
+  </si>
+  <si>
+    <t>236.85 segundos</t>
+  </si>
+  <si>
+    <t>238.38 segundos</t>
+  </si>
+  <si>
+    <t>235.16 segundos</t>
+  </si>
+  <si>
+    <t>236.61 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 232.39 segundos</t>
+  </si>
+  <si>
+    <t>236.31 segundos</t>
+  </si>
+  <si>
+    <t>239.81 segundos</t>
+  </si>
+  <si>
+    <t>233.41 segundos</t>
+  </si>
+  <si>
+    <t>217.14 segundos</t>
+  </si>
+  <si>
+    <t>221.56 segundos</t>
+  </si>
+  <si>
+    <t>216.07 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 212.43 segundos</t>
+  </si>
+  <si>
+    <t>215.37 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 224.46 segundos</t>
+  </si>
+  <si>
+    <t>253.82 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 262.36 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 254.73 segundos</t>
+  </si>
+  <si>
+    <t>261.58 segundos</t>
+  </si>
+  <si>
+    <t>252.60 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 259.10 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 254.85 segundos</t>
+  </si>
+  <si>
+    <t>257.08 segundos</t>
+  </si>
+  <si>
+    <t>238.21 segundos</t>
+  </si>
+  <si>
+    <t>255.94 segundos</t>
+  </si>
+  <si>
+    <t>251.97 segundos</t>
+  </si>
+  <si>
+    <t>255.42 segundos</t>
+  </si>
+  <si>
+    <t>254.62 segundos</t>
+  </si>
+  <si>
+    <t>261.19 segundos</t>
+  </si>
+  <si>
+    <t>251.65 segundos</t>
+  </si>
+  <si>
+    <t>240.48 segundos</t>
+  </si>
+  <si>
+    <t>244.98 segundos</t>
   </si>
 </sst>
 </file>
@@ -515,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75374EE-7030-44B4-A324-43D055AB0147}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -526,52 +634,1118 @@
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="13.1328125" customWidth="1"/>
     <col min="5" max="5" width="11.9296875" customWidth="1"/>
+    <col min="7" max="7" width="15.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
+      <c r="B2">
+        <v>466</v>
+      </c>
+      <c r="C2">
+        <v>44000</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>303</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1">
-        <v>5.2083333333333336E-2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B3">
+        <v>418</v>
+      </c>
+      <c r="C3">
+        <v>43000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>310</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <v>408</v>
+      </c>
+      <c r="C4">
+        <v>42000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>309</v>
+      </c>
+      <c r="F4">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <v>398</v>
+      </c>
+      <c r="C5">
+        <v>41000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>291</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>389</v>
+      </c>
+      <c r="C6">
+        <v>40000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>306</v>
+      </c>
+      <c r="F6">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <v>379</v>
+      </c>
+      <c r="C7">
+        <v>39000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>300</v>
+      </c>
+      <c r="F7">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>369</v>
+      </c>
+      <c r="C8">
+        <v>38000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>304</v>
+      </c>
+      <c r="F8">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <v>359</v>
+      </c>
+      <c r="C9">
+        <v>37000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>298</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>350</v>
+      </c>
+      <c r="C10">
+        <v>36000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>300</v>
+      </c>
+      <c r="F10">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <v>340</v>
+      </c>
+      <c r="C11">
+        <v>35000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>303</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <v>330</v>
+      </c>
+      <c r="C12">
+        <v>34000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>298</v>
+      </c>
+      <c r="F12">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <v>320</v>
+      </c>
+      <c r="C13">
+        <v>33000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>305</v>
+      </c>
+      <c r="F13">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>311</v>
+      </c>
+      <c r="C14">
+        <v>32000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>302</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B15">
+        <v>301</v>
+      </c>
+      <c r="C15">
+        <v>31000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>308</v>
+      </c>
+      <c r="F15">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B16">
+        <v>291</v>
+      </c>
+      <c r="C16">
+        <v>30000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>305</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B17">
+        <v>282</v>
+      </c>
+      <c r="C17">
+        <v>29000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>301</v>
+      </c>
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <v>272</v>
+      </c>
+      <c r="C18">
+        <v>28000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>301</v>
+      </c>
+      <c r="F18">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B19">
+        <v>262</v>
+      </c>
+      <c r="C19">
+        <v>27000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>305</v>
+      </c>
+      <c r="F19">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B20">
+        <v>252</v>
+      </c>
+      <c r="C20">
+        <v>26000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>306</v>
+      </c>
+      <c r="F20">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B21">
+        <v>243</v>
+      </c>
+      <c r="C21">
+        <v>25000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21">
+        <v>299</v>
+      </c>
+      <c r="F21">
+        <v>15</v>
+      </c>
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B22">
+        <v>233</v>
+      </c>
+      <c r="C22">
+        <v>24000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22">
+        <v>305</v>
+      </c>
+      <c r="F22">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B23">
+        <v>223</v>
+      </c>
+      <c r="C23">
+        <v>23000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>305</v>
+      </c>
+      <c r="F23">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B24">
+        <v>213</v>
+      </c>
+      <c r="C24">
+        <v>22000</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24">
+        <v>305</v>
+      </c>
+      <c r="F24">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B25">
+        <v>204</v>
+      </c>
+      <c r="C25">
+        <v>21000</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>311</v>
+      </c>
+      <c r="F25">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B26">
+        <v>194</v>
+      </c>
+      <c r="C26">
+        <v>20000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>307</v>
+      </c>
+      <c r="F26">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B27">
+        <v>184</v>
+      </c>
+      <c r="C27">
+        <v>19000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>300</v>
+      </c>
+      <c r="F27">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B28">
+        <v>175</v>
+      </c>
+      <c r="C28">
+        <v>18000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>299</v>
+      </c>
+      <c r="F28">
+        <v>14</v>
+      </c>
+      <c r="G28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <v>165</v>
+      </c>
+      <c r="C29">
+        <v>17000</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>300</v>
+      </c>
+      <c r="F29">
+        <v>14</v>
+      </c>
+      <c r="G29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>155</v>
+      </c>
+      <c r="C30">
+        <v>16000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30">
+        <v>307</v>
+      </c>
+      <c r="F30">
+        <v>13</v>
+      </c>
+      <c r="G30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B31">
+        <v>145</v>
+      </c>
+      <c r="C31">
+        <v>15000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>302</v>
+      </c>
+      <c r="F31">
+        <v>13</v>
+      </c>
+      <c r="G31" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" t="s">
+        <v>31</v>
+      </c>
+      <c r="J31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <v>136</v>
+      </c>
+      <c r="C32">
+        <v>14000</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>296</v>
+      </c>
+      <c r="F32">
+        <v>13</v>
+      </c>
+      <c r="G32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B33">
+        <v>126</v>
+      </c>
+      <c r="C33">
+        <v>13000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33">
+        <v>340</v>
+      </c>
+      <c r="F33">
+        <v>13</v>
+      </c>
+      <c r="G33" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" t="s">
+        <v>31</v>
+      </c>
+      <c r="J33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <v>116</v>
+      </c>
+      <c r="C34">
+        <v>12000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>334</v>
+      </c>
+      <c r="F34">
+        <v>13</v>
+      </c>
+      <c r="G34" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B35">
+        <v>106</v>
+      </c>
+      <c r="C35">
+        <v>11000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>316</v>
+      </c>
+      <c r="F35">
+        <v>13</v>
+      </c>
+      <c r="G35" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" t="s">
+        <v>31</v>
+      </c>
+      <c r="J35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B36">
+        <v>97</v>
+      </c>
+      <c r="C36">
+        <v>10000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>332</v>
+      </c>
+      <c r="F36">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
+        <v>69</v>
+      </c>
+      <c r="H36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36" t="s">
+        <v>31</v>
+      </c>
+      <c r="J36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B37">
+        <v>87</v>
+      </c>
+      <c r="C37">
+        <v>9000</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37">
+        <v>339</v>
+      </c>
+      <c r="F37">
+        <v>13</v>
+      </c>
+      <c r="G37" t="s">
+        <v>70</v>
+      </c>
+      <c r="H37" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" t="s">
+        <v>31</v>
+      </c>
+      <c r="J37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B38">
+        <v>77</v>
+      </c>
+      <c r="C38">
+        <v>8000</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>347</v>
+      </c>
+      <c r="F38">
+        <v>14</v>
+      </c>
+      <c r="G38" t="s">
+        <v>71</v>
+      </c>
+      <c r="H38" t="s">
+        <v>31</v>
+      </c>
+      <c r="I38" t="s">
+        <v>31</v>
+      </c>
+      <c r="J38" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -582,10 +1756,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FB3867-F72D-4725-8F36-56B7E0614DBC}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -598,68 +1772,71 @@
     <col min="8" max="8" width="13.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1.6</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>963</v>
       </c>
@@ -667,28 +1844,28 @@
         <v>31000</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>932</v>
       </c>
@@ -696,28 +1873,28 @@
         <v>30000</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>901</v>
       </c>
@@ -725,28 +1902,28 @@
         <v>29000</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>870</v>
       </c>
@@ -754,28 +1931,28 @@
         <v>28000</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>838</v>
       </c>
@@ -783,28 +1960,28 @@
         <v>27000</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>807</v>
       </c>
@@ -812,28 +1989,28 @@
         <v>26000</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>776</v>
       </c>
@@ -841,28 +2018,28 @@
         <v>25000</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>745</v>
       </c>
@@ -870,28 +2047,28 @@
         <v>24000</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>714</v>
       </c>
@@ -899,7 +2076,7 @@
         <v>23000</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E11">
         <v>1481</v>
@@ -908,19 +2085,22 @@
         <v>30</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" t="s">
         <v>34</v>
       </c>
-      <c r="I11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>683</v>
       </c>
@@ -928,7 +2108,7 @@
         <v>22000</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E12">
         <v>1449</v>
@@ -937,19 +2117,22 @@
         <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" t="s">
         <v>34</v>
       </c>
-      <c r="I12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>652</v>
       </c>
@@ -957,7 +2140,7 @@
         <v>21000</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <v>1430</v>
@@ -966,19 +2149,22 @@
         <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" t="s">
         <v>34</v>
       </c>
-      <c r="I13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>621</v>
       </c>
@@ -986,7 +2172,7 @@
         <v>20000</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>1464</v>
@@ -995,19 +2181,22 @@
         <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" t="s">
         <v>34</v>
       </c>
-      <c r="I14" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>590</v>
       </c>
@@ -1015,7 +2204,7 @@
         <v>19000</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E15">
         <v>1451</v>
@@ -1024,19 +2213,22 @@
         <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" t="s">
         <v>34</v>
       </c>
-      <c r="I15" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>559</v>
       </c>
@@ -1044,7 +2236,7 @@
         <v>18000</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E16">
         <v>1480</v>
@@ -1053,19 +2245,22 @@
         <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" t="s">
         <v>34</v>
       </c>
-      <c r="I16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>528</v>
       </c>
@@ -1073,7 +2268,7 @@
         <v>17000</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E17">
         <v>1448</v>
@@ -1082,19 +2277,22 @@
         <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" t="s">
         <v>34</v>
       </c>
-      <c r="I17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>497</v>
       </c>
@@ -1102,7 +2300,7 @@
         <v>16000</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E18">
         <v>1460</v>
@@ -1111,19 +2309,22 @@
         <v>30</v>
       </c>
       <c r="G18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" t="s">
         <v>34</v>
       </c>
-      <c r="I18" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>466</v>
       </c>
@@ -1131,7 +2332,7 @@
         <v>15000</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E19">
         <v>1453</v>
@@ -1140,19 +2341,22 @@
         <v>26</v>
       </c>
       <c r="G19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" t="s">
+        <v>31</v>
+      </c>
+      <c r="L19" t="s">
         <v>34</v>
       </c>
-      <c r="I19" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>435</v>
       </c>
@@ -1160,7 +2364,7 @@
         <v>14000</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E20">
         <v>1504</v>
@@ -1169,19 +2373,22 @@
         <v>32</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" t="s">
         <v>34</v>
       </c>
-      <c r="I20" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>403</v>
       </c>
@@ -1189,7 +2396,7 @@
         <v>13000</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E21">
         <v>1703</v>
@@ -1198,19 +2405,22 @@
         <v>26</v>
       </c>
       <c r="G21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21" t="s">
         <v>34</v>
       </c>
-      <c r="I21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>372</v>
       </c>
@@ -1218,7 +2428,7 @@
         <v>12000</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E22">
         <v>1708</v>
@@ -1227,19 +2437,22 @@
         <v>33</v>
       </c>
       <c r="G22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" t="s">
         <v>34</v>
       </c>
-      <c r="I22" t="s">
-        <v>34</v>
-      </c>
-      <c r="J22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>341</v>
       </c>
@@ -1247,7 +2460,7 @@
         <v>11000</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E23">
         <v>1673</v>
@@ -1256,19 +2469,22 @@
         <v>30</v>
       </c>
       <c r="G23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L23" t="s">
         <v>34</v>
       </c>
-      <c r="I23" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>310</v>
       </c>
@@ -1276,7 +2492,7 @@
         <v>10000</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E24">
         <v>1713</v>
@@ -1285,19 +2501,22 @@
         <v>26</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24" t="s">
         <v>34</v>
       </c>
-      <c r="I24" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>279</v>
       </c>
@@ -1305,7 +2524,7 @@
         <v>9000</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E25">
         <v>1805</v>
@@ -1314,19 +2533,22 @@
         <v>18</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25" t="s">
+        <v>31</v>
+      </c>
+      <c r="L25" t="s">
         <v>34</v>
       </c>
-      <c r="I25" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>248</v>
       </c>
@@ -1334,7 +2556,7 @@
         <v>8000</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E26">
         <v>1994</v>
@@ -1343,15 +2565,18 @@
         <v>24</v>
       </c>
       <c r="G26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J26" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>